<commit_message>
Update to include detector hall parameters and output file
</commit_message>
<xml_diff>
--- a/11-Parameters/nuSTORM-PrdStrght-Params-v1.0.xlsx
+++ b/11-Parameters/nuSTORM-PrdStrght-Params-v1.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/CubMac-Home/Neutrinos/nuSTORM/19-Sw/01-Local/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/CubMac-Home/Neutrinos/nuSTORM/19-Sw/03-nuSTORM/nuSTORM/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2225F4C3-BB98-8245-A59F-16F5C5900138}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EEB6FE-0A35-4243-857C-F44F49BCABB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="28040" windowHeight="17440" xr2:uid="{A18852C7-9E71-0140-BF5E-AC1F94132CB3}"/>
+    <workbookView xWindow="16540" yWindow="5160" windowWidth="28040" windowHeight="17440" xr2:uid="{A18852C7-9E71-0140-BF5E-AC1F94132CB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -91,6 +91,30 @@
   </si>
   <si>
     <t>nuSIM-2021-01</t>
+  </si>
+  <si>
+    <t>Distance from end of straighg to detector hall</t>
+  </si>
+  <si>
+    <t>HallWallDist</t>
+  </si>
+  <si>
+    <t>DetHlfWdth</t>
+  </si>
+  <si>
+    <t>Detector half width</t>
+  </si>
+  <si>
+    <t>Detector length</t>
+  </si>
+  <si>
+    <t>DetLngth</t>
+  </si>
+  <si>
+    <t>Distance from hall wall to detector entrance</t>
+  </si>
+  <si>
+    <t>Hall2Det</t>
   </si>
 </sst>
 </file>
@@ -451,15 +475,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0649E6B0-F0C3-944D-8FF8-0186EE602342}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -566,6 +590,74 @@
         <v>18</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>